<commit_message>
Updated the view definitions as well as '0002_create_views.py'.
</commit_message>
<xml_diff>
--- a/b11_1/pgsql/views/views.xlsx
+++ b/b11_1/pgsql/views/views.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yann/Prog/Python/LBA/b11_1/pgsql/views/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02B1079-4DE0-7949-BA90-BDEC4FB63EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5050D284-0BC1-6C46-8D9E-12737CD12E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7880" yWindow="6200" windowWidth="41020" windowHeight="16440" xr2:uid="{6B16D59E-6A66-4A47-81CB-8E6A71CFF365}"/>
+    <workbookView xWindow="7860" yWindow="6200" windowWidth="41020" windowHeight="16440" xr2:uid="{6B16D59E-6A66-4A47-81CB-8E6A71CFF365}"/>
   </bookViews>
   <sheets>
     <sheet name="MARA - Grunddaten" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <externalReferences>
     <externalReference r:id="rId10"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
   <si>
     <t>SOURCE_ID</t>
   </si>
@@ -243,6 +243,12 @@
   <si>
     <t>CLASS</t>
   </si>
+  <si>
+    <t>MARA-MHDRZ</t>
+  </si>
+  <si>
+    <t>MARA-IPRKZ</t>
+  </si>
 </sst>
 </file>
 
@@ -257,12 +263,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -277,8 +289,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -321,6 +334,7 @@
       <sheetName val="MARC - Werksdaten"/>
       <sheetName val="MVKE - Verkaufsdaten"/>
       <sheetName val="MBEW - Buchhaltung"/>
+      <sheetName val="CKMLCR - Material-Ledger-Preise"/>
       <sheetName val="MARA_AUSP - Merkmale"/>
       <sheetName val="MARA_KSSK - Klassenzuordnung"/>
       <sheetName val="MLAN - Steuer"/>
@@ -333,251 +347,247 @@
             <v>Positions-Nr.</v>
           </cell>
           <cell r="C5" t="str">
-            <v>Referenz-Nr.
-Lieferant</v>
+            <v>Kurztext DE</v>
           </cell>
           <cell r="D5" t="str">
-            <v>Kurztext DE</v>
+            <v>Kurztext FR</v>
           </cell>
           <cell r="E5" t="str">
-            <v>Kurztext FR</v>
+            <v>Kurztext EN</v>
           </cell>
           <cell r="F5" t="str">
-            <v>Kurztext EN</v>
+            <v>Grunddatentext DE - 1. Zeile</v>
           </cell>
           <cell r="G5" t="str">
-            <v>Grunddatentext DE - 1. Zeile</v>
+            <v>Grunddatentext DE - 2. Zeile</v>
           </cell>
           <cell r="H5" t="str">
-            <v>Grunddatentext DE - 2. Zeile</v>
+            <v>Grunddatentext FR - 1. Zeile</v>
           </cell>
           <cell r="I5" t="str">
-            <v>Grunddatentext FR - 1. Zeile</v>
+            <v>Grunddatentext FR - 2. Zeile</v>
           </cell>
           <cell r="J5" t="str">
-            <v>Grunddatentext FR - 2. Zeile</v>
+            <v>Grunddatentext EN - 1. Zeile</v>
           </cell>
           <cell r="K5" t="str">
-            <v>Grunddatentext EN - 1. Zeile</v>
+            <v>Grunddatentext EN - 2. Zeile</v>
           </cell>
           <cell r="L5" t="str">
-            <v>Grunddatentext EN - 2. Zeile</v>
-          </cell>
-          <cell r="M5" t="str">
             <v>Basis-
 Mengeneinheit</v>
           </cell>
-          <cell r="N5" t="str">
+          <cell r="M5" t="str">
             <v>Brutto-
 gewicht</v>
           </cell>
-          <cell r="O5" t="str">
+          <cell r="N5" t="str">
             <v>Gewichts-
 einheit</v>
           </cell>
-          <cell r="P5" t="str">
+          <cell r="O5" t="str">
             <v>Netto-
 gewicht</v>
           </cell>
+          <cell r="P5" t="str">
+            <v>Grösse / Abmessung</v>
+          </cell>
           <cell r="Q5" t="str">
-            <v>Grösse / Abmessung</v>
+            <v>EAN / UPC Code</v>
           </cell>
           <cell r="R5" t="str">
-            <v>EAN / UPC Code</v>
-          </cell>
-          <cell r="S5" t="str">
             <v>Nato Stock
 Number</v>
           </cell>
-          <cell r="T5" t="str">
+          <cell r="S5" t="str">
             <v>NSN
 Gruppe / Klasse</v>
           </cell>
-          <cell r="U5" t="str">
+          <cell r="T5" t="str">
             <v>Nato
 Versorgungs-Nr.</v>
           </cell>
+          <cell r="U5" t="str">
+            <v>Herstellerteilenummer</v>
+          </cell>
           <cell r="V5" t="str">
-            <v>Herstellerteilenummer</v>
+            <v>Normbezeichnung</v>
           </cell>
           <cell r="W5" t="str">
-            <v>Normbezeichnung</v>
+            <v>Gefahrgutkennzeichen</v>
           </cell>
           <cell r="X5" t="str">
-            <v>Gefahrgutkennzeichen</v>
-          </cell>
-          <cell r="Y5" t="str">
             <v>Instand-
 setzbar</v>
           </cell>
-          <cell r="Z5" t="str">
+          <cell r="Y5" t="str">
             <v>Chargen-
 pflicht</v>
           </cell>
-          <cell r="AA5" t="str">
+          <cell r="Z5" t="str">
             <v>Bestell-
 mengeneinheit</v>
           </cell>
-          <cell r="AB5" t="str">
+          <cell r="AA5" t="str">
             <v>Mindest-
 bestellmenge</v>
           </cell>
+          <cell r="AB5" t="str">
+            <v>Lieferzeit</v>
+          </cell>
           <cell r="AC5" t="str">
-            <v>Lieferzeit</v>
-          </cell>
-          <cell r="AD5" t="str">
             <v>Einheit
 L / B / H</v>
           </cell>
+          <cell r="AD5" t="str">
+            <v>Länge</v>
+          </cell>
           <cell r="AE5" t="str">
-            <v>Länge</v>
+            <v>Breite</v>
           </cell>
           <cell r="AF5" t="str">
-            <v>Breite</v>
+            <v>Höhe</v>
           </cell>
           <cell r="AG5" t="str">
-            <v>Höhe</v>
+            <v>Preis</v>
           </cell>
           <cell r="AH5" t="str">
-            <v>Preis</v>
+            <v>Währung</v>
           </cell>
           <cell r="AI5" t="str">
-            <v>Währung</v>
-          </cell>
-          <cell r="AJ5" t="str">
             <v>Preis-
 einheit</v>
           </cell>
+          <cell r="AJ5" t="str">
+            <v>Lagerfähigkeit</v>
+          </cell>
           <cell r="AK5" t="str">
-            <v>Lagerfähigkeit</v>
-          </cell>
-          <cell r="AL5" t="str">
             <v>Export-
 kontrollauflage</v>
           </cell>
+          <cell r="AL5" t="str">
+            <v>CAGE Code</v>
+          </cell>
           <cell r="AM5" t="str">
-            <v>CAGE Code</v>
+            <v>Hersteller Name</v>
           </cell>
           <cell r="AN5" t="str">
-            <v>Hersteller Name</v>
+            <v>Hersteller Adresse</v>
           </cell>
           <cell r="AO5" t="str">
-            <v>Hersteller Adresse</v>
+            <v xml:space="preserve">Hersteller PLZ </v>
           </cell>
           <cell r="AP5" t="str">
-            <v xml:space="preserve">Hersteller PLZ </v>
+            <v>Hersteller Ort</v>
           </cell>
           <cell r="AQ5" t="str">
-            <v>Hersteller Ort</v>
+            <v>Revision</v>
           </cell>
           <cell r="AR5" t="str">
-            <v>Revision</v>
-          </cell>
-          <cell r="AS5" t="str">
             <v>Bemerkung</v>
           </cell>
         </row>
         <row r="8">
+          <cell r="C8" t="str">
+            <v>MAKTX1</v>
+          </cell>
           <cell r="D8" t="str">
-            <v>MAKTX1</v>
+            <v>MAKTX2</v>
           </cell>
           <cell r="E8" t="str">
-            <v>MAKTX2</v>
+            <v>MAKTX3</v>
           </cell>
           <cell r="F8" t="str">
-            <v>MAKTX3</v>
+            <v>TDLINE1</v>
           </cell>
           <cell r="G8" t="str">
-            <v>TDLINE1</v>
+            <v>TDLINE1-2</v>
           </cell>
           <cell r="H8" t="str">
-            <v>TDLINE1-2</v>
+            <v>TDLINE2</v>
           </cell>
           <cell r="I8" t="str">
-            <v>TDLINE2</v>
+            <v>TDLINE2-2</v>
           </cell>
           <cell r="J8" t="str">
-            <v>TDLINE2-2</v>
+            <v>TDLINE3</v>
           </cell>
           <cell r="K8" t="str">
-            <v>TDLINE3</v>
+            <v>TDLINE3-2</v>
           </cell>
           <cell r="L8" t="str">
-            <v>TDLINE3-2</v>
+            <v>MEINS</v>
           </cell>
           <cell r="M8" t="str">
-            <v>MEINS</v>
+            <v>BRGEW</v>
           </cell>
           <cell r="N8" t="str">
-            <v>BRGEW</v>
+            <v>GEWEI</v>
           </cell>
           <cell r="O8" t="str">
-            <v>GEWEI</v>
+            <v>NTGEW</v>
           </cell>
           <cell r="P8" t="str">
-            <v>NTGEW</v>
+            <v>GROES</v>
           </cell>
           <cell r="Q8" t="str">
-            <v>GROES</v>
-          </cell>
-          <cell r="R8" t="str">
             <v>EAN11</v>
           </cell>
+          <cell r="S8" t="str">
+            <v>NSNID-Gruppe</v>
+          </cell>
           <cell r="T8" t="str">
-            <v>NSNID-Gruppe</v>
+            <v>NSNID</v>
           </cell>
           <cell r="U8" t="str">
-            <v>NSNID</v>
+            <v>MFRPN</v>
           </cell>
           <cell r="V8" t="str">
-            <v>MFRPN</v>
+            <v>NORMT</v>
           </cell>
           <cell r="W8" t="str">
-            <v>NORMT</v>
+            <v>PROFL</v>
           </cell>
           <cell r="X8" t="str">
-            <v>PROFL</v>
+            <v>SPC_H</v>
           </cell>
           <cell r="Y8" t="str">
-            <v>SPC_H</v>
+            <v>XCHPF</v>
           </cell>
           <cell r="Z8" t="str">
-            <v>XCHPF</v>
+            <v>BSTME</v>
           </cell>
           <cell r="AA8" t="str">
-            <v>BSTME</v>
+            <v>BSTMI</v>
           </cell>
           <cell r="AB8" t="str">
-            <v>BSTMI</v>
+            <v>PLIFZ</v>
           </cell>
           <cell r="AC8" t="str">
-            <v>PLIFZ</v>
+            <v>MEABM</v>
           </cell>
           <cell r="AD8" t="str">
-            <v>MEABM</v>
+            <v>LAENG</v>
           </cell>
           <cell r="AE8" t="str">
-            <v>LAENG</v>
+            <v>BREIT</v>
           </cell>
           <cell r="AF8" t="str">
-            <v>BREIT</v>
+            <v>HOEHE</v>
           </cell>
           <cell r="AG8" t="str">
-            <v>HOEHE</v>
+            <v>V_BEWERTUNGSPREIS</v>
           </cell>
           <cell r="AH8" t="str">
-            <v>V_BEWERTUNGSPREIS</v>
+            <v>V_WAEHRUNG</v>
           </cell>
           <cell r="AI8" t="str">
-            <v>V_WAEHRUNG</v>
+            <v>V_PREISEINHEIT</v>
           </cell>
           <cell r="AJ8" t="str">
-            <v>V_PREISEINHEIT</v>
+            <v>V_LAGERFAEHIGKEIT</v>
           </cell>
           <cell r="AK8" t="str">
-            <v>MARA-MHDHB</v>
-          </cell>
-          <cell r="AL8" t="str">
             <v>EXPORT_H</v>
           </cell>
         </row>
@@ -594,59 +604,58 @@
             <v>BEGRU</v>
           </cell>
           <cell r="D5" t="str">
+            <v>Sparte</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>Geschäftspartner</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v xml:space="preserve">Warengruppe </v>
+          </cell>
+          <cell r="G5" t="str">
+            <v>Übersetzungsstatus</v>
+          </cell>
+          <cell r="H5" t="str">
+            <v>Verteilung an PSD</v>
+          </cell>
+          <cell r="I5" t="str">
+            <v>Revision
+Eigen</v>
+          </cell>
+          <cell r="J5" t="str">
+            <v>Zertifiziert
+für Flug</v>
+          </cell>
+          <cell r="K5" t="str">
+            <v>Verteilung an RUAG</v>
+          </cell>
+          <cell r="L5" t="str">
+            <v>Revision
+Fremd</v>
+          </cell>
+          <cell r="M5" t="str">
+            <v>A-Nummer</v>
+          </cell>
+          <cell r="N5" t="str">
             <v xml:space="preserve">
 Materialart
 (Grunddaten)
 </v>
           </cell>
-          <cell r="E5" t="str">
-            <v>Sparte</v>
-          </cell>
-          <cell r="F5" t="str">
+          <cell r="O5" t="str">
             <v>Produkthierarchie</v>
           </cell>
-          <cell r="G5" t="str">
+          <cell r="P5" t="str">
+            <v>Rückführungscode</v>
+          </cell>
+          <cell r="Q5" t="str">
+            <v>Serialnummerprofil</v>
+          </cell>
+          <cell r="R5" t="str">
+            <v>Endbevorratet</v>
+          </cell>
+          <cell r="S5" t="str">
             <v>Materialzustandsverwaltung</v>
-          </cell>
-          <cell r="H5" t="str">
-            <v>Rückführungscode</v>
-          </cell>
-          <cell r="I5" t="str">
-            <v>Serialnummerprofil</v>
-          </cell>
-          <cell r="J5" t="str">
-            <v>Hersteller-Nr.
-(GP)</v>
-          </cell>
-          <cell r="K5" t="str">
-            <v xml:space="preserve">Warengruppe </v>
-          </cell>
-          <cell r="L5" t="str">
-            <v>Übersetzungsstatus</v>
-          </cell>
-          <cell r="M5" t="str">
-            <v>Endbevorratet</v>
-          </cell>
-          <cell r="N5" t="str">
-            <v>Revision
-Fremd</v>
-          </cell>
-          <cell r="O5" t="str">
-            <v>Revision
-Eigen</v>
-          </cell>
-          <cell r="P5" t="str">
-            <v>Zertifiziert
-für Flug</v>
-          </cell>
-          <cell r="Q5" t="str">
-            <v>A-Nummer</v>
-          </cell>
-          <cell r="R5" t="str">
-            <v>Verteilung an PSD</v>
-          </cell>
-          <cell r="S5" t="str">
-            <v>Verteilung an RUAG</v>
           </cell>
         </row>
         <row r="8">
@@ -654,52 +663,52 @@
             <v>BEGRU</v>
           </cell>
           <cell r="D8" t="str">
+            <v>SPART</v>
+          </cell>
+          <cell r="E8" t="str">
+            <v>MFRNR</v>
+          </cell>
+          <cell r="F8" t="str">
+            <v>MATKL</v>
+          </cell>
+          <cell r="G8" t="str">
+            <v>V_UEBERSETZUNG</v>
+          </cell>
+          <cell r="H8" t="str">
+            <v>V_VERTEILUNG_PSD</v>
+          </cell>
+          <cell r="I8" t="str">
+            <v>V_Reveigen</v>
+          </cell>
+          <cell r="J8" t="str">
+            <v>V_ZERTFLUG</v>
+          </cell>
+          <cell r="K8" t="str">
+            <v>V_VERTEILUNG_RUAG</v>
+          </cell>
+          <cell r="L8" t="str">
+            <v>V_REVFREMD</v>
+          </cell>
+          <cell r="M8" t="str">
+            <v>V_A_NUMMER</v>
+          </cell>
+          <cell r="N8" t="str">
             <v>MTART</v>
           </cell>
-          <cell r="E8" t="str">
-            <v>SPART</v>
-          </cell>
-          <cell r="F8" t="str">
+          <cell r="O8" t="str">
             <v>PRDHA</v>
           </cell>
-          <cell r="G8" t="str">
+          <cell r="P8" t="str">
+            <v>RETDELC</v>
+          </cell>
+          <cell r="Q8" t="str">
+            <v>SERNP</v>
+          </cell>
+          <cell r="R8" t="str">
+            <v>V_ENDBEVORRATET</v>
+          </cell>
+          <cell r="S8" t="str">
             <v>MCOND</v>
-          </cell>
-          <cell r="H8" t="str">
-            <v>RETDELC</v>
-          </cell>
-          <cell r="I8" t="str">
-            <v>SERNP</v>
-          </cell>
-          <cell r="J8" t="str">
-            <v>MFRNR</v>
-          </cell>
-          <cell r="K8" t="str">
-            <v>MATKL</v>
-          </cell>
-          <cell r="L8" t="str">
-            <v>V_UEBERSETZUNG</v>
-          </cell>
-          <cell r="M8" t="str">
-            <v>V_ENDBEVORRATET</v>
-          </cell>
-          <cell r="N8" t="str">
-            <v>V_REVFREMD</v>
-          </cell>
-          <cell r="O8" t="str">
-            <v>V_Reveigen</v>
-          </cell>
-          <cell r="P8" t="str">
-            <v>V_ZERTFLUG</v>
-          </cell>
-          <cell r="Q8" t="str">
-            <v>V_A_NUMMER</v>
-          </cell>
-          <cell r="R8" t="str">
-            <v>V_VERTEILUNG_PSD</v>
-          </cell>
-          <cell r="S8" t="str">
-            <v>V_VERTEILUNG_RUAG</v>
           </cell>
         </row>
       </sheetData>
@@ -712,162 +721,171 @@
             <v>Kurztext DE</v>
           </cell>
           <cell r="C5" t="str">
-            <v>Werkszuordnung (1)</v>
+            <v>Werkszuordnung</v>
           </cell>
           <cell r="D5" t="str">
-            <v>Werkszuordnung (2)</v>
+            <v>Werkszuordnung (2) - Info</v>
           </cell>
           <cell r="E5" t="str">
-            <v>Werkszuordnung (3)</v>
+            <v>Werkszuordnung (3) - Info</v>
           </cell>
           <cell r="F5" t="str">
-            <v>Werkszuordnung (4)</v>
+            <v>Werkszuordnung (4) - Info</v>
           </cell>
           <cell r="G5" t="str">
             <v>Allgemeine Positionstypengruppe</v>
           </cell>
           <cell r="H5" t="str">
+            <v>Spare Part Class Code</v>
+          </cell>
+          <cell r="I5" t="str">
+            <v>Fertigungssteuerer</v>
+          </cell>
+          <cell r="J5" t="str">
+            <v>Sonderablauf</v>
+          </cell>
+          <cell r="K5" t="str">
+            <v>Temperaturbedingung</v>
+          </cell>
+          <cell r="L5" t="str">
+            <v>Systemmanager</v>
+          </cell>
+          <cell r="M5" t="str">
+            <v>Mietrelevanz</v>
+          </cell>
+          <cell r="N5" t="str">
+            <v>Nachschubklasse</v>
+          </cell>
+          <cell r="O5" t="str">
+            <v>Materialeinstufung nach ZUVA</v>
+          </cell>
+          <cell r="P5" t="str">
+            <v>Orderbuchpflicht</v>
+          </cell>
+          <cell r="Q5" t="str">
+            <v>Verteilung APM Kerda</v>
+          </cell>
+          <cell r="R5" t="str">
+            <v>Verteilung SVSAA</v>
+          </cell>
+          <cell r="S5" t="str">
+            <v>Verteilung CHEOPS</v>
+          </cell>
+          <cell r="T5" t="str">
+            <v>Zuteilung</v>
+          </cell>
+          <cell r="U5" t="str">
+            <v>Ausprägung</v>
+          </cell>
+          <cell r="V5" t="str">
             <v>Verkaufsorg.</v>
           </cell>
-          <cell r="I5" t="str">
+          <cell r="W5" t="str">
             <v>Vertriebsweg</v>
           </cell>
-          <cell r="J5" t="str">
+          <cell r="X5" t="str">
+            <v>Auszeichnungsfeld</v>
+          </cell>
+          <cell r="Y5" t="str">
+            <v>Preissteuerung</v>
+          </cell>
+          <cell r="Z5" t="str">
+            <v>Preisermittlung</v>
+          </cell>
+          <cell r="AA5" t="str">
+            <v>Bewertungsklasse</v>
+          </cell>
+          <cell r="AB5" t="str">
             <v>Führendes Material</v>
           </cell>
-          <cell r="K5" t="str">
-            <v>Auszeichnungsfeld</v>
-          </cell>
-          <cell r="L5" t="str">
-            <v>CPV-Code</v>
-          </cell>
-          <cell r="M5" t="str">
-            <v>Spare Part Class Code</v>
-          </cell>
-          <cell r="N5" t="str">
-            <v>Fertigungssteuerer</v>
-          </cell>
-          <cell r="O5" t="str">
+          <cell r="AC5" t="str">
             <v>Kennzeichen komplexes System</v>
           </cell>
-          <cell r="P5" t="str">
-            <v>Sonderablauf</v>
-          </cell>
-          <cell r="Q5" t="str">
-            <v>Temperaturbedingung</v>
-          </cell>
-          <cell r="R5" t="str">
-            <v>Bewertungsklasse</v>
-          </cell>
-          <cell r="S5" t="str">
-            <v>Systemmanager</v>
-          </cell>
-          <cell r="T5" t="str">
+          <cell r="AD5" t="str">
             <v>Kennziffer BAMF</v>
           </cell>
-          <cell r="U5" t="str">
-            <v>Mietrelevanz</v>
-          </cell>
-          <cell r="V5" t="str">
+          <cell r="AE5" t="str">
             <v>Next Higher Assembly</v>
-          </cell>
-          <cell r="W5" t="str">
-            <v>Nachschubklasse</v>
-          </cell>
-          <cell r="X5" t="str">
-            <v>Verteilung APM Kerda</v>
-          </cell>
-          <cell r="Y5" t="str">
-            <v>Verteilung SVSAA</v>
-          </cell>
-          <cell r="Z5" t="str">
-            <v>Verteilung CHEOPS</v>
-          </cell>
-          <cell r="AA5" t="str">
-            <v>Zuteilung</v>
-          </cell>
-          <cell r="AB5" t="str">
-            <v>Ausprägung</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8" t="str">
-            <v>WERKS_1</v>
-          </cell>
-          <cell r="D8" t="str">
-            <v>WERKS_2</v>
-          </cell>
-          <cell r="E8" t="str">
-            <v>WERKS_3</v>
-          </cell>
-          <cell r="F8" t="str">
-            <v>WERKS_4</v>
+            <v>WERKS</v>
           </cell>
           <cell r="G8" t="str">
             <v>MTPOS</v>
           </cell>
           <cell r="H8" t="str">
+            <v>ADSPC_SPC</v>
+          </cell>
+          <cell r="I8" t="str">
+            <v>FEVOR</v>
+          </cell>
+          <cell r="J8" t="str">
+            <v>ZZSONDERABLAUF</v>
+          </cell>
+          <cell r="K8" t="str">
+            <v>TEMPB</v>
+          </cell>
+          <cell r="L8" t="str">
+            <v>V_Systemmanager</v>
+          </cell>
+          <cell r="M8" t="str">
+            <v>V_MIET_RELEVANZ</v>
+          </cell>
+          <cell r="N8" t="str">
+            <v>V_NACHSCHUBKLASSE</v>
+          </cell>
+          <cell r="O8" t="str">
+            <v>HNDLCODE</v>
+          </cell>
+          <cell r="P8" t="str">
+            <v>KORDB</v>
+          </cell>
+          <cell r="Q8" t="str">
+            <v>V_APM</v>
+          </cell>
+          <cell r="R8" t="str">
+            <v>V_SVSAA</v>
+          </cell>
+          <cell r="S8" t="str">
+            <v>V_CHEOPS</v>
+          </cell>
+          <cell r="T8" t="str">
+            <v>Zuteilung</v>
+          </cell>
+          <cell r="U8" t="str">
+            <v>Ausprägung</v>
+          </cell>
+          <cell r="V8" t="str">
             <v>VKORG</v>
           </cell>
-          <cell r="I8" t="str">
+          <cell r="W8" t="str">
             <v>VTWEG</v>
           </cell>
-          <cell r="J8" t="str">
+          <cell r="X8" t="str">
+            <v>ZZLABEL</v>
+          </cell>
+          <cell r="Y8" t="str">
+            <v>VPRSV</v>
+          </cell>
+          <cell r="Z8" t="str">
+            <v>MLAST</v>
+          </cell>
+          <cell r="AA8" t="str">
+            <v>BKLAS</v>
+          </cell>
+          <cell r="AB8" t="str">
             <v>ZZFUEHR_MAT</v>
           </cell>
-          <cell r="K8" t="str">
-            <v>ZZLABEL</v>
-          </cell>
-          <cell r="L8" t="str">
-            <v>ZZCPVCODE</v>
-          </cell>
-          <cell r="M8" t="str">
-            <v>ADSPC_SPC</v>
-          </cell>
-          <cell r="N8" t="str">
-            <v>FEVOR</v>
-          </cell>
-          <cell r="O8" t="str">
+          <cell r="AC8" t="str">
             <v>ZZIHKOMP</v>
           </cell>
-          <cell r="P8" t="str">
-            <v>ZZSONDERABLAUF</v>
-          </cell>
-          <cell r="Q8" t="str">
-            <v>TEMPB</v>
-          </cell>
-          <cell r="R8" t="str">
-            <v>BKLAS</v>
-          </cell>
-          <cell r="S8" t="str">
-            <v>V_Systemmanager</v>
-          </cell>
-          <cell r="T8" t="str">
+          <cell r="AD8" t="str">
             <v>V_KENNZIFFER</v>
           </cell>
-          <cell r="U8" t="str">
-            <v>V_MIET_RELEVANZ</v>
-          </cell>
-          <cell r="V8" t="str">
+          <cell r="AE8" t="str">
             <v>V_NEXT_HIGHER</v>
-          </cell>
-          <cell r="W8" t="str">
-            <v>V_NACHSCHUBKLASSE</v>
-          </cell>
-          <cell r="X8" t="str">
-            <v>V_APM</v>
-          </cell>
-          <cell r="Y8" t="str">
-            <v>V_SVSAA</v>
-          </cell>
-          <cell r="Z8" t="str">
-            <v>V_CHEOPS</v>
-          </cell>
-          <cell r="AA8" t="str">
-            <v>Zuteilung</v>
-          </cell>
-          <cell r="AB8" t="str">
-            <v>Ausprägung</v>
           </cell>
         </row>
       </sheetData>
@@ -890,6 +908,7 @@
       <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1212,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E2A3DB-E416-FA44-864C-F849214D90D9}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1336,8 +1355,7 @@
       </c>
       <c r="C6" t="str">
         <f>_xlfn.IFNA(INDEX([1]Grunddaten!$5:$5,MATCH(A6,[1]Grunddaten!$8:$8,0)),"")</f>
-        <v>Hersteller-Nr.
-(GP)</v>
+        <v>Geschäftspartner</v>
       </c>
       <c r="D6" t="str">
         <f>_xlfn.IFNA(INDEX('[1]Systemmanager - Datenassistent'!$5:$5,MATCH(A6,'[1]Systemmanager - Datenassistent'!$8:$8,0)),"")</f>
@@ -1345,8 +1363,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>Hersteller-Nr.
-(GP)</v>
+        <v>Geschäftspartner</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1567,23 +1584,23 @@
         <v>EAN / UPC Code</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17" s="1" t="str">
         <f>_xlfn.IFNA(INDEX([1]Input_Lieferant!$5:$5, MATCH(A17, [1]Input_Lieferant!$8:$8,0)),"")</f>
         <v/>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="1" t="str">
         <f>_xlfn.IFNA(INDEX([1]Grunddaten!$5:$5,MATCH(A17,[1]Grunddaten!$8:$8,0)),"")</f>
         <v/>
       </c>
-      <c r="D17" t="str">
+      <c r="D17" s="1" t="str">
         <f>_xlfn.IFNA(INDEX('[1]Systemmanager - Datenassistent'!$5:$5,MATCH(A17,'[1]Systemmanager - Datenassistent'!$8:$8,0)),"")</f>
         <v/>
       </c>
-      <c r="E17" t="str">
+      <c r="E17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
@@ -1630,23 +1647,23 @@
         <v>Normbezeichnung</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="str">
+      <c r="B20" s="1" t="str">
         <f>_xlfn.IFNA(INDEX([1]Input_Lieferant!$5:$5, MATCH(A20, [1]Input_Lieferant!$8:$8,0)),"")</f>
         <v/>
       </c>
-      <c r="C20" t="str">
+      <c r="C20" s="1" t="str">
         <f>_xlfn.IFNA(INDEX([1]Grunddaten!$5:$5,MATCH(A20,[1]Grunddaten!$8:$8,0)),"")</f>
         <v/>
       </c>
-      <c r="D20" t="str">
+      <c r="D20" s="1" t="str">
         <f>_xlfn.IFNA(INDEX('[1]Systemmanager - Datenassistent'!$5:$5,MATCH(A20,'[1]Systemmanager - Datenassistent'!$8:$8,0)),"")</f>
         <v/>
       </c>
-      <c r="E20" t="str">
+      <c r="E20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
@@ -1783,23 +1800,23 @@
 pflicht</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="str">
+      <c r="B27" s="1" t="str">
         <f>_xlfn.IFNA(INDEX([1]Input_Lieferant!$5:$5, MATCH(A27, [1]Input_Lieferant!$8:$8,0)),"")</f>
         <v/>
       </c>
-      <c r="C27" t="str">
+      <c r="C27" s="1" t="str">
         <f>_xlfn.IFNA(INDEX([1]Grunddaten!$5:$5,MATCH(A27,[1]Grunddaten!$8:$8,0)),"")</f>
         <v/>
       </c>
-      <c r="D27" t="str">
+      <c r="D27" s="1" t="str">
         <f>_xlfn.IFNA(INDEX('[1]Systemmanager - Datenassistent'!$5:$5,MATCH(A27,'[1]Systemmanager - Datenassistent'!$8:$8,0)),"")</f>
         <v/>
       </c>
-      <c r="E27" t="str">
+      <c r="E27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
@@ -1951,25 +1968,25 @@
         <v>Produkthierarchie</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35" t="str">
+      <c r="B35" s="1" t="str">
         <f>_xlfn.IFNA(INDEX([1]Input_Lieferant!$5:$5, MATCH(A35, [1]Input_Lieferant!$8:$8,0)),"")</f>
         <v/>
       </c>
-      <c r="C35" t="str">
+      <c r="C35" s="1" t="str">
         <f>_xlfn.IFNA(INDEX([1]Grunddaten!$5:$5,MATCH(A35,[1]Grunddaten!$8:$8,0)),"")</f>
         <v/>
       </c>
-      <c r="D35" t="str">
+      <c r="D35" s="1" t="str">
         <f>_xlfn.IFNA(INDEX('[1]Systemmanager - Datenassistent'!$5:$5,MATCH(A35,'[1]Systemmanager - Datenassistent'!$8:$8,0)),"")</f>
-        <v/>
-      </c>
-      <c r="E35" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>Materialeinstufung nach ZUVA</v>
+      </c>
+      <c r="E35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Materialeinstufung nach ZUVA</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -2007,11 +2024,11 @@
       </c>
       <c r="D37" t="str">
         <f>_xlfn.IFNA(INDEX('[1]Systemmanager - Datenassistent'!$5:$5,MATCH(A37,'[1]Systemmanager - Datenassistent'!$8:$8,0)),"")</f>
-        <v>CPV-Code</v>
+        <v/>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v>CPV-Code</v>
+        <v>-</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2041,7 +2058,7 @@
       </c>
       <c r="B39" t="str">
         <f>_xlfn.IFNA(INDEX([1]Input_Lieferant!$5:$5, MATCH(A39, [1]Input_Lieferant!$8:$8,0)),"")</f>
-        <v>Lagerfähigkeit</v>
+        <v/>
       </c>
       <c r="C39" t="str">
         <f>_xlfn.IFNA(INDEX([1]Grunddaten!$5:$5,MATCH(A39,[1]Grunddaten!$8:$8,0)),"")</f>
@@ -2053,7 +2070,49 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
-        <v>Lagerfähigkeit</v>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="1" t="str">
+        <f>_xlfn.IFNA(INDEX([1]Input_Lieferant!$5:$5, MATCH(A40, [1]Input_Lieferant!$8:$8,0)),"")</f>
+        <v/>
+      </c>
+      <c r="C40" s="1" t="str">
+        <f>_xlfn.IFNA(INDEX([1]Grunddaten!$5:$5,MATCH(A40,[1]Grunddaten!$8:$8,0)),"")</f>
+        <v/>
+      </c>
+      <c r="D40" s="1" t="str">
+        <f>_xlfn.IFNA(INDEX('[1]Systemmanager - Datenassistent'!$5:$5,MATCH(A40,'[1]Systemmanager - Datenassistent'!$8:$8,0)),"")</f>
+        <v/>
+      </c>
+      <c r="E40" s="1" t="str">
+        <f t="shared" ref="E40:E41" si="1">IF(LEN(B40&amp;C40&amp;D40)=0,"-",_xlfn.CONCAT(B40,C40,D40))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="1" t="str">
+        <f>_xlfn.IFNA(INDEX([1]Input_Lieferant!$5:$5, MATCH(A41, [1]Input_Lieferant!$8:$8,0)),"")</f>
+        <v/>
+      </c>
+      <c r="C41" s="1" t="str">
+        <f>_xlfn.IFNA(INDEX([1]Grunddaten!$5:$5,MATCH(A41,[1]Grunddaten!$8:$8,0)),"")</f>
+        <v/>
+      </c>
+      <c r="D41" s="1" t="str">
+        <f>_xlfn.IFNA(INDEX('[1]Systemmanager - Datenassistent'!$5:$5,MATCH(A41,'[1]Systemmanager - Datenassistent'!$8:$8,0)),"")</f>
+        <v/>
+      </c>
+      <c r="E41" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
       </c>
     </row>
   </sheetData>
@@ -3516,7 +3575,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4307,11 +4366,11 @@
       </c>
       <c r="D3" t="str">
         <f>_xlfn.IFNA(INDEX('[1]Systemmanager - Datenassistent'!$5:$5,MATCH(A3,'[1]Systemmanager - Datenassistent'!$8:$8,0)),"")</f>
-        <v/>
+        <v>Werkszuordnung</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E39" si="0">IF(LEN(B3&amp;C3&amp;D3)=0,"-",_xlfn.CONCAT(B3,C3,D3))</f>
-        <v>-</v>
+        <v>Werkszuordnung</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>